<commit_message>
Test und Training Data Sets
:)
</commit_message>
<xml_diff>
--- a/Missing_and_Variable_Selection/RF-Summaries.xlsx
+++ b/Missing_and_Variable_Selection/RF-Summaries.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="0" windowWidth="26240" windowHeight="16800" tabRatio="500"/>
+    <workbookView xWindow="8860" yWindow="0" windowWidth="17720" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -590,18 +590,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -619,20 +613,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -964,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1022,7 +1019,7 @@
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
@@ -1052,7 +1049,7 @@
       <c r="K2">
         <v>579.43597750608205</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="N2">
@@ -1069,7 +1066,7 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -1099,7 +1096,7 @@
       <c r="K3">
         <v>417.402820284386</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N3">
@@ -1116,7 +1113,7 @@
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -1146,7 +1143,7 @@
       <c r="K4">
         <v>268.25467345454098</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="N4">
@@ -1163,7 +1160,7 @@
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">
@@ -1193,7 +1190,7 @@
       <c r="K5">
         <v>225.49450698644699</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="N5">
@@ -1210,7 +1207,7 @@
       </c>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6">
@@ -1240,7 +1237,7 @@
       <c r="K6">
         <v>370.992422661555</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N6">
@@ -1257,7 +1254,7 @@
       </c>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7">
@@ -1287,7 +1284,7 @@
       <c r="K7">
         <v>279.761978045207</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="N7">
@@ -1304,7 +1301,7 @@
       </c>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8">
@@ -1334,7 +1331,7 @@
       <c r="K8">
         <v>332.05441781194401</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N8">
@@ -1351,7 +1348,7 @@
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9">
@@ -1381,7 +1378,7 @@
       <c r="K9">
         <v>213.63991944382499</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="N9">
@@ -1398,7 +1395,7 @@
       </c>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10">
@@ -1428,7 +1425,7 @@
       <c r="K10">
         <v>271.21546549022599</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="N10">
@@ -1445,7 +1442,7 @@
       </c>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11">
@@ -1475,7 +1472,7 @@
       <c r="K11">
         <v>217.76611666909801</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N11">
@@ -1492,7 +1489,7 @@
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12">
@@ -1522,7 +1519,7 @@
       <c r="K12">
         <v>235.14033294092999</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="N12">
@@ -1539,7 +1536,7 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13">
@@ -1569,7 +1566,7 @@
       <c r="K13">
         <v>105.54546394883501</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="N13">
@@ -1586,7 +1583,7 @@
       </c>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14">
@@ -1633,7 +1630,7 @@
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15">
@@ -1663,7 +1660,7 @@
       <c r="K15">
         <v>249.67895418818901</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N15">
@@ -1680,7 +1677,7 @@
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16">
@@ -1727,7 +1724,7 @@
       </c>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17">
@@ -1774,7 +1771,7 @@
       </c>
     </row>
     <row r="18" spans="1:17">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B18">
@@ -1804,7 +1801,7 @@
       <c r="K18">
         <v>239.25068155425001</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N18">
@@ -1821,7 +1818,7 @@
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B19">
@@ -1868,7 +1865,7 @@
       </c>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B20">
@@ -1898,7 +1895,7 @@
       <c r="K20">
         <v>242.00196597978399</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="2" t="s">
         <v>21</v>
       </c>
       <c r="N20">
@@ -1915,7 +1912,7 @@
       </c>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B21">
@@ -1945,7 +1942,7 @@
       <c r="K21">
         <v>206.64727639003499</v>
       </c>
-      <c r="M21" t="s">
+      <c r="M21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N21">
@@ -1962,7 +1959,7 @@
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B22">
@@ -2009,7 +2006,7 @@
       </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B23">
@@ -2039,7 +2036,7 @@
       <c r="K23">
         <v>234.62980561710901</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="N23">
@@ -2056,7 +2053,7 @@
       </c>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B24">
@@ -2086,7 +2083,7 @@
       <c r="K24">
         <v>215.278517506741</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N24">
@@ -2103,7 +2100,7 @@
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B25">
@@ -2133,7 +2130,7 @@
       <c r="K25">
         <v>174.10366191395701</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N25">
@@ -2150,7 +2147,7 @@
       </c>
     </row>
     <row r="26" spans="1:17">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B26">
@@ -2180,7 +2177,7 @@
       <c r="K26">
         <v>185.03070155447199</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="2" t="s">
         <v>28</v>
       </c>
       <c r="N26">
@@ -2227,7 +2224,7 @@
       <c r="K27">
         <v>234.076973478599</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="N27">
@@ -2274,7 +2271,7 @@
       <c r="K28">
         <v>230.122515853983</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="2" t="s">
         <v>36</v>
       </c>
       <c r="N28">
@@ -2321,7 +2318,7 @@
       <c r="K29">
         <v>134.70753916640601</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="N29">
@@ -2368,7 +2365,7 @@
       <c r="K30">
         <v>172.90521213241101</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="2" t="s">
         <v>29</v>
       </c>
       <c r="N30">
@@ -2415,7 +2412,7 @@
       <c r="K31">
         <v>138.65244357072999</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="2" t="s">
         <v>38</v>
       </c>
       <c r="N31">

</xml_diff>